<commit_message>
Changed the applications icon, report update
</commit_message>
<xml_diff>
--- a/Sprint Backlog/SprintBacklog2nd.xlsx
+++ b/Sprint Backlog/SprintBacklog2nd.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="55">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -282,35 +282,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="56">
     <dxf>
       <fill>
         <patternFill>
@@ -1010,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,9 +1247,7 @@
       <c r="G12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1307,6 +1277,12 @@
       <c r="E13">
         <v>4</v>
       </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1321,6 +1297,12 @@
       <c r="E14">
         <v>5</v>
       </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1335,6 +1317,12 @@
       <c r="E15">
         <v>2</v>
       </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1349,6 +1337,12 @@
       <c r="E16">
         <v>4</v>
       </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1443,7 +1437,7 @@
         <v>6</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1483,6 +1477,9 @@
       <c r="F24">
         <v>12</v>
       </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1500,6 +1497,9 @@
       <c r="F25">
         <v>8</v>
       </c>
+      <c r="G25">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1520,6 +1520,9 @@
       <c r="F26">
         <v>6</v>
       </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
@@ -1578,6 +1581,9 @@
       <c r="F30">
         <v>12</v>
       </c>
+      <c r="G30">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -1595,6 +1601,9 @@
       <c r="F31">
         <v>4</v>
       </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1615,8 +1624,11 @@
       <c r="F32" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1632,8 +1644,11 @@
       <c r="F33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1649,8 +1664,11 @@
       <c r="F34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1666,8 +1684,11 @@
       <c r="F35" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1683,8 +1704,11 @@
       <c r="F36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1700,8 +1724,11 @@
       <c r="F37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1717,8 +1744,11 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1734,8 +1764,11 @@
       <c r="F39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1751,8 +1784,11 @@
       <c r="F40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1768,8 +1804,11 @@
       <c r="F41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1785,8 +1824,11 @@
       <c r="F42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1802,8 +1844,11 @@
       <c r="F43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1819,234 +1864,253 @@
       <c r="F44">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
+      <c r="B46">
+        <f>SUM(B5:B44)</f>
+        <v>121</v>
+      </c>
+      <c r="E46">
+        <f>SUM(E5:E44)</f>
+        <v>101</v>
+      </c>
+      <c r="F46">
+        <f>SUM(F5:F44)</f>
+        <v>98</v>
+      </c>
+      <c r="G46">
+        <f>SUM(G5:G44)</f>
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="59" priority="54" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="55" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="56" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="56" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D9">
-    <cfRule type="containsText" dxfId="55" priority="50" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="51" priority="50" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="51" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="49" priority="52" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D9">
-    <cfRule type="cellIs" dxfId="52" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="51" priority="46" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="47" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D16">
-    <cfRule type="containsText" dxfId="47" priority="42" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="43" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="41" priority="44" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D16">
-    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="containsText" dxfId="43" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="39" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="39" priority="34" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="35" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="36" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="35" priority="30" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="32" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D33">
-    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="27" priority="26" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="25" priority="28" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D33">
-    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="27" priority="22" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="23" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D37">
-    <cfRule type="containsText" dxfId="23" priority="18" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="19" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D37">
-    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:D41">
-    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:D41">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42:D44">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42:D44">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",D26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>